<commit_message>
Update scripts and report template
</commit_message>
<xml_diff>
--- a/files/NEW_UAL_OJS_Report_Template.xlsx
+++ b/files/NEW_UAL_OJS_Report_Template.xlsx
@@ -437,11 +437,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1788541259"/>
-        <c:axId val="700070012"/>
+        <c:axId val="787283407"/>
+        <c:axId val="1379148371"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1788541259"/>
+        <c:axId val="787283407"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -493,10 +493,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="700070012"/>
+        <c:crossAx val="1379148371"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="700070012"/>
+        <c:axId val="1379148371"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -572,7 +572,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1788541259"/>
+        <c:crossAx val="787283407"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -730,11 +730,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="553590713"/>
-        <c:axId val="1997485158"/>
+        <c:axId val="1531108283"/>
+        <c:axId val="603591567"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="553590713"/>
+        <c:axId val="1531108283"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -786,10 +786,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1997485158"/>
+        <c:crossAx val="603591567"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1997485158"/>
+        <c:axId val="603591567"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -865,7 +865,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="553590713"/>
+        <c:crossAx val="1531108283"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>

</xml_diff>